<commit_message>
Completed galaxy import implementation
</commit_message>
<xml_diff>
--- a/Data/JISA -- transactions.xlsx
+++ b/Data/JISA -- transactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Portfolio-management\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Y\Portfolio management\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257DA2F9-D1FF-443D-9815-00B8C81C497B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970281D7-B5CD-45E4-B3DA-D8FC8477806F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{135C7015-3CD8-41F8-B453-0698FCF992B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{135C7015-3CD8-41F8-B453-0698FCF992B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Транзакции_JISA" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="Restricted">[1]Портфель!$G$12</definedName>
     <definedName name="Unrestricted">[1]Портфель!$G$11</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,16 +81,10 @@
     <t>HSBC FTSE 250 Index Accumulation C</t>
   </si>
   <si>
-    <t>Vanguard U.S. Equity Index Fund GBP Acc</t>
-  </si>
-  <si>
     <t>GB00BJS8SH10</t>
   </si>
   <si>
     <t>GB00B80QG052</t>
-  </si>
-  <si>
-    <t>GB00B5B71Q71</t>
   </si>
   <si>
     <t>Количество</t>
@@ -196,6 +190,12 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>Test security</t>
+  </si>
+  <si>
+    <t>TESTISIN322223</t>
   </si>
 </sst>
 </file>
@@ -661,15 +661,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>791633</xdr:colOff>
+          <xdr:colOff>790575</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>46567</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>122767</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -679,7 +679,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93AC1D43-F234-487E-8B13-3E124DAB9785}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -701,14 +701,14 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="54864" tIns="41148" rIns="54864" bIns="41148" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="27432" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -728,7 +728,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Портфель"/>
@@ -937,6 +937,7 @@
       <sheetName val="Result_Sterling"/>
       <sheetName val="CF_Sterling"/>
       <sheetName val="Транзакции_Sterling"/>
+      <sheetName val="Galaxy_2201 v16"/>
     </sheetNames>
     <definedNames>
       <definedName name="Coms_JISA"/>
@@ -963,7 +964,13 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="5">
+        <row r="17">
+          <cell r="BG17">
+            <v>41946</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
@@ -1041,7 +1048,13 @@
       <sheetData sheetId="74"/>
       <sheetData sheetId="75"/>
       <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
+      <sheetData sheetId="77">
+        <row r="163">
+          <cell r="B163">
+            <v>44264</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="78"/>
       <sheetData sheetId="79"/>
       <sheetData sheetId="80"/>
@@ -1085,7 +1098,13 @@
       <sheetData sheetId="118"/>
       <sheetData sheetId="119"/>
       <sheetData sheetId="120"/>
-      <sheetData sheetId="121"/>
+      <sheetData sheetId="121">
+        <row r="30">
+          <cell r="T30">
+            <v>41934</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="122"/>
       <sheetData sheetId="123"/>
       <sheetData sheetId="124"/>
@@ -1170,6 +1189,7 @@
       <sheetData sheetId="203"/>
       <sheetData sheetId="204"/>
       <sheetData sheetId="205"/>
+      <sheetData sheetId="206" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1475,54 +1495,56 @@
   <sheetPr codeName="Sheet95"/>
   <dimension ref="A1:AL53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" outlineLevelRow="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.64453125" customWidth="1"/>
-    <col min="3" max="3" width="2.76171875" customWidth="1"/>
-    <col min="4" max="4" width="11.64453125" customWidth="1"/>
-    <col min="5" max="5" width="9.41015625" customWidth="1"/>
-    <col min="6" max="6" width="6.5859375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.29296875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.8203125" customWidth="1"/>
-    <col min="12" max="12" width="11.64453125" customWidth="1"/>
-    <col min="13" max="13" width="9.41015625" customWidth="1"/>
-    <col min="14" max="14" width="6.5859375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.29296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="7" customWidth="1"/>
-    <col min="18" max="18" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="1.8203125" customWidth="1"/>
-    <col min="20" max="20" width="11.64453125" customWidth="1"/>
-    <col min="21" max="21" width="9.41015625" customWidth="1"/>
-    <col min="22" max="22" width="6.5859375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.29296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.85546875" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" customWidth="1"/>
+    <col min="22" max="22" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" style="1" customWidth="1"/>
     <col min="25" max="25" width="7" customWidth="1"/>
-    <col min="26" max="26" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.76171875" style="2" customWidth="1"/>
-    <col min="28" max="28" width="11.64453125" customWidth="1"/>
-    <col min="29" max="29" width="9.41015625" customWidth="1"/>
-    <col min="30" max="30" width="6.5859375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.29296875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.7109375" style="2" customWidth="1"/>
+    <col min="28" max="28" width="11.7109375" customWidth="1"/>
+    <col min="29" max="29" width="9.42578125" customWidth="1"/>
+    <col min="30" max="30" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.28515625" style="1" customWidth="1"/>
     <col min="33" max="33" width="7" customWidth="1"/>
-    <col min="34" max="34" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="9.76171875" customWidth="1"/>
-    <col min="37" max="37" width="11.1171875" customWidth="1"/>
-    <col min="38" max="38" width="2.76171875" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="9.7109375" customWidth="1"/>
+    <col min="37" max="37" width="11.140625" customWidth="1"/>
+    <col min="38" max="38" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AA1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1547,7 +1569,7 @@
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
@@ -1569,12 +1591,12 @@
       <c r="AK2" s="3"/>
       <c r="AL2" s="3"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -1584,7 +1606,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="3"/>
       <c r="L3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1594,7 +1616,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="3"/>
       <c r="T3" s="5" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
@@ -1603,7 +1625,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
       <c r="AB3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
@@ -1616,50 +1638,50 @@
       <c r="AK3" s="5"/>
       <c r="AL3" s="3"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
       <c r="I4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J4" s="10">
         <v>1667.2127663648409</v>
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="R4" s="10">
         <v>3737.0851084758692</v>
       </c>
       <c r="S4" s="10"/>
       <c r="T4" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Z4" s="10">
         <v>12.925085276847049</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
@@ -1669,7 +1691,7 @@
         <v>310.07359325257369</v>
       </c>
       <c r="AI4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AJ4" s="10">
         <v>310.07359325257369</v>
@@ -1679,12 +1701,12 @@
       </c>
       <c r="AL4" s="7"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1698,7 +1720,7 @@
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -1712,7 +1734,7 @@
       </c>
       <c r="S5" s="10"/>
       <c r="T5" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
@@ -1725,7 +1747,7 @@
         <v>5525.18</v>
       </c>
       <c r="AB5" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
@@ -1746,7 +1768,7 @@
       </c>
       <c r="AL5" s="7"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>44926</v>
       </c>
@@ -1795,12 +1817,12 @@
       <c r="AK6" s="15"/>
       <c r="AL6" s="7"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1811,7 +1833,7 @@
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -1822,7 +1844,7 @@
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
@@ -1842,47 +1864,47 @@
       <c r="AK7" s="10"/>
       <c r="AL7" s="7"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="20"/>
       <c r="C8" s="7"/>
       <c r="D8" s="21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="23"/>
       <c r="G8" s="23"/>
       <c r="H8" s="24"/>
       <c r="I8" s="25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J8" s="18">
         <v>3.6411000000000002</v>
       </c>
       <c r="K8" s="10"/>
       <c r="L8" s="21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M8" s="22"/>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
       <c r="P8" s="24"/>
       <c r="Q8" s="25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="R8" s="18">
         <v>3.42</v>
       </c>
       <c r="S8" s="10"/>
       <c r="T8" s="21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="U8" s="22"/>
       <c r="V8" s="23"/>
       <c r="W8" s="23"/>
       <c r="X8" s="24"/>
       <c r="Y8" s="25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Z8" s="18">
         <v>776.14</v>
@@ -1898,22 +1920,22 @@
       <c r="AK8" s="10"/>
       <c r="AL8" s="7"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="26">
         <v>0</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
       <c r="H9" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I9" s="30" t="e">
         <v>#DIV/0!</v>
@@ -1923,13 +1945,13 @@
       </c>
       <c r="K9" s="10"/>
       <c r="L9" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M9" s="28"/>
       <c r="N9" s="28"/>
       <c r="O9" s="28"/>
       <c r="P9" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Q9" s="30" t="e">
         <v>#DIV/0!</v>
@@ -1939,13 +1961,13 @@
       </c>
       <c r="S9" s="10"/>
       <c r="T9" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="U9" s="28"/>
       <c r="V9" s="28"/>
       <c r="W9" s="28"/>
       <c r="X9" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Y9" s="30" t="e">
         <v>#DIV/0!</v>
@@ -1965,16 +1987,16 @@
       <c r="AK9" s="31"/>
       <c r="AL9" s="7"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="35">
         <v>0</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1990,7 +2012,7 @@
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -2006,7 +2028,7 @@
       </c>
       <c r="S10" s="10"/>
       <c r="T10" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
@@ -2032,16 +2054,16 @@
       <c r="AK10" s="10"/>
       <c r="AL10" s="7"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="35">
         <v>0</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -2055,7 +2077,7 @@
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -2069,7 +2091,7 @@
       </c>
       <c r="S11" s="10"/>
       <c r="T11" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
@@ -2093,16 +2115,16 @@
       <c r="AK11" s="10"/>
       <c r="AL11" s="7"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="26">
         <v>0</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -2116,7 +2138,7 @@
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -2130,7 +2152,7 @@
       </c>
       <c r="S12" s="10"/>
       <c r="T12" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
@@ -2154,16 +2176,16 @@
       <c r="AK12" s="10"/>
       <c r="AL12" s="7"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="26">
         <v>0</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -2177,7 +2199,7 @@
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -2191,7 +2213,7 @@
       </c>
       <c r="S13" s="10"/>
       <c r="T13" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
@@ -2215,10 +2237,10 @@
       <c r="AK13" s="10"/>
       <c r="AL13" s="7"/>
     </row>
-    <row r="14" spans="1:38" s="39" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:38" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
@@ -2232,7 +2254,7 @@
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M14" s="23"/>
       <c r="N14" s="23"/>
@@ -2246,7 +2268,7 @@
       </c>
       <c r="S14" s="10"/>
       <c r="T14" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U14" s="23"/>
       <c r="V14" s="23"/>
@@ -2271,11 +2293,11 @@
       <c r="AK14" s="41"/>
       <c r="AL14" s="7"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="C15" s="42"/>
       <c r="D15" s="43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" s="44"/>
       <c r="F15" s="44"/>
@@ -2287,7 +2309,7 @@
       </c>
       <c r="K15" s="47"/>
       <c r="L15" s="43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M15" s="44"/>
       <c r="N15" s="44"/>
@@ -2299,7 +2321,7 @@
       </c>
       <c r="S15" s="47"/>
       <c r="T15" s="43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U15" s="44"/>
       <c r="V15" s="44"/>
@@ -2322,12 +2344,12 @@
       <c r="AK15" s="47"/>
       <c r="AL15" s="42"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2339,7 +2361,7 @@
       </c>
       <c r="K16" s="51"/>
       <c r="L16" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -2351,7 +2373,7 @@
       </c>
       <c r="S16" s="51"/>
       <c r="T16" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
@@ -2372,14 +2394,14 @@
       <c r="AK16" s="51"/>
       <c r="AL16" s="7"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="7"/>
       <c r="D17" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -2389,7 +2411,7 @@
       <c r="J17" s="14"/>
       <c r="K17" s="16"/>
       <c r="L17" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
@@ -2399,7 +2421,7 @@
       <c r="R17" s="14"/>
       <c r="S17" s="16"/>
       <c r="T17" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U17" s="13"/>
       <c r="V17" s="13"/>
@@ -2408,7 +2430,7 @@
       <c r="Y17" s="13"/>
       <c r="Z17" s="14"/>
       <c r="AB17" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AC17" s="13"/>
       <c r="AD17" s="13"/>
@@ -2421,12 +2443,12 @@
       <c r="AK17" s="15"/>
       <c r="AL17" s="7"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -2437,7 +2459,7 @@
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -2448,7 +2470,7 @@
       </c>
       <c r="S18" s="10"/>
       <c r="T18" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
@@ -2458,7 +2480,7 @@
         <v>427.47725695066475</v>
       </c>
       <c r="AB18" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
@@ -2476,50 +2498,50 @@
       </c>
       <c r="AL18" s="7"/>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="4"/>
       <c r="I19" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J19" s="18">
         <v>3.6411000000000002</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="R19" s="18">
         <v>3.42</v>
       </c>
       <c r="S19" s="10"/>
       <c r="T19" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Z19" s="18">
         <v>776.14</v>
       </c>
       <c r="AB19" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
@@ -2529,7 +2551,7 @@
         <v>1.9809813327110899</v>
       </c>
       <c r="AI19" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AJ19" s="18">
         <v>2.644610079169305</v>
@@ -2539,22 +2561,22 @@
       </c>
       <c r="AL19" s="7"/>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" s="26">
         <v>8779.1851613705621</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I20" s="53">
         <v>0.20182980748499268</v>
@@ -2564,13 +2586,13 @@
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M20" s="28"/>
       <c r="N20" s="28"/>
       <c r="O20" s="28"/>
       <c r="P20" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Q20" s="53">
         <v>4.9521082858736687E-2</v>
@@ -2580,13 +2602,13 @@
       </c>
       <c r="S20" s="10"/>
       <c r="T20" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="U20" s="28"/>
       <c r="V20" s="28"/>
       <c r="W20" s="28"/>
       <c r="X20" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Y20" s="53">
         <v>8.6399793019474647E-2</v>
@@ -2595,7 +2617,7 @@
         <v>4506.4956867720684</v>
       </c>
       <c r="AB20" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC20" s="28"/>
       <c r="AD20" s="28"/>
@@ -2616,16 +2638,16 @@
       </c>
       <c r="AL20" s="7"/>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="35">
         <v>14.269999999999847</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -2641,7 +2663,7 @@
       </c>
       <c r="K21" s="10"/>
       <c r="L21" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -2657,7 +2679,7 @@
       </c>
       <c r="S21" s="10"/>
       <c r="T21" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
@@ -2672,7 +2694,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
@@ -2691,16 +2713,16 @@
       </c>
       <c r="AL21" s="7"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="35">
         <v>8764.9151613705617</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -2714,7 +2736,7 @@
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -2728,7 +2750,7 @@
       </c>
       <c r="S22" s="10"/>
       <c r="T22" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
@@ -2741,7 +2763,7 @@
         <v>4506.4956867720684</v>
       </c>
       <c r="AB22" s="34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
@@ -2760,16 +2782,16 @@
       </c>
       <c r="AL22" s="7"/>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" s="26">
         <v>0</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -2783,7 +2805,7 @@
       </c>
       <c r="K23" s="10"/>
       <c r="L23" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -2797,7 +2819,7 @@
       </c>
       <c r="S23" s="10"/>
       <c r="T23" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -2810,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="AB23" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
@@ -2829,16 +2851,16 @@
       </c>
       <c r="AL23" s="7"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" s="26">
         <v>0</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -2852,7 +2874,7 @@
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -2866,7 +2888,7 @@
       </c>
       <c r="S24" s="10"/>
       <c r="T24" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
@@ -2879,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="AB24" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
@@ -2898,12 +2920,12 @@
       </c>
       <c r="AL24" s="7"/>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
@@ -2917,7 +2939,7 @@
       </c>
       <c r="K25" s="10"/>
       <c r="L25" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M25" s="23"/>
       <c r="N25" s="23"/>
@@ -2931,7 +2953,7 @@
       </c>
       <c r="S25" s="10"/>
       <c r="T25" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U25" s="23"/>
       <c r="V25" s="23"/>
@@ -2944,7 +2966,7 @@
         <v>4506.4956867720684</v>
       </c>
       <c r="AB25" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AC25" s="23"/>
       <c r="AD25" s="23"/>
@@ -2963,12 +2985,12 @@
       </c>
       <c r="AL25" s="7"/>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="42"/>
       <c r="B26" s="42"/>
       <c r="C26" s="42"/>
       <c r="D26" s="43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E26" s="44"/>
       <c r="F26" s="44"/>
@@ -2980,7 +3002,7 @@
       </c>
       <c r="K26" s="47"/>
       <c r="L26" s="43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M26" s="44"/>
       <c r="N26" s="44"/>
@@ -2992,7 +3014,7 @@
       </c>
       <c r="S26" s="47"/>
       <c r="T26" s="43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U26" s="44"/>
       <c r="V26" s="44"/>
@@ -3004,7 +3026,7 @@
       </c>
       <c r="AA26" s="48"/>
       <c r="AB26" s="42" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC26" s="49"/>
       <c r="AD26" s="49"/>
@@ -3023,12 +3045,12 @@
       </c>
       <c r="AL26" s="42"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="26"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -3040,7 +3062,7 @@
       </c>
       <c r="K27" s="51"/>
       <c r="L27" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
@@ -3052,7 +3074,7 @@
       </c>
       <c r="S27" s="51"/>
       <c r="T27" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
@@ -3063,7 +3085,7 @@
         <v>0.16986168026924134</v>
       </c>
       <c r="AB27" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
@@ -3081,7 +3103,7 @@
       </c>
       <c r="AL27" s="7"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -3115,102 +3137,102 @@
       <c r="AH28" s="3"/>
       <c r="AL28" s="3"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="55"/>
       <c r="B29" s="55"/>
       <c r="C29" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="57" t="s">
+      <c r="F29" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="G29" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="57" t="s">
+      <c r="H29" s="58" t="s">
         <v>27</v>
-      </c>
-      <c r="G29" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="58" t="s">
-        <v>29</v>
       </c>
       <c r="I29" s="58"/>
       <c r="J29" s="57" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K29" s="55"/>
       <c r="L29" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="M29" s="57" t="s">
+      <c r="O29" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="N29" s="57" t="s">
+      <c r="P29" s="58" t="s">
         <v>27</v>
-      </c>
-      <c r="O29" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="P29" s="58" t="s">
-        <v>29</v>
       </c>
       <c r="Q29" s="58"/>
       <c r="R29" s="57" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S29" s="55"/>
       <c r="T29" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="U29" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="V29" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="U29" s="57" t="s">
+      <c r="W29" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="V29" s="57" t="s">
+      <c r="X29" s="58" t="s">
         <v>27</v>
-      </c>
-      <c r="W29" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="X29" s="58" t="s">
-        <v>29</v>
       </c>
       <c r="Y29" s="58"/>
       <c r="Z29" s="57" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AB29" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC29" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD29" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="AC29" s="57" t="s">
+      <c r="AE29" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="AD29" s="57" t="s">
+      <c r="AF29" s="58" t="s">
         <v>27</v>
-      </c>
-      <c r="AE29" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF29" s="58" t="s">
-        <v>29</v>
       </c>
       <c r="AG29" s="58"/>
       <c r="AH29" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI29" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ29" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="AI29" s="57" t="s">
+      <c r="AK29" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AJ29" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK29" s="57" t="s">
-        <v>33</v>
-      </c>
       <c r="AL29" s="55"/>
     </row>
-    <row r="30" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="59"/>
       <c r="B30" s="59"/>
       <c r="C30">
@@ -3273,7 +3295,7 @@
       </c>
       <c r="AL30" s="64"/>
     </row>
-    <row r="31" spans="1:38" s="71" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:38" s="71" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="70"/>
       <c r="B31" s="70"/>
       <c r="C31" s="71">
@@ -3331,7 +3353,7 @@
       <c r="AK31" s="35"/>
       <c r="AL31" s="77"/>
     </row>
-    <row r="32" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="59"/>
       <c r="B32" s="60"/>
       <c r="C32">
@@ -3388,7 +3410,7 @@
       <c r="AK32" s="62"/>
       <c r="AL32" s="60"/>
     </row>
-    <row r="33" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
       <c r="C33">
@@ -3445,7 +3467,7 @@
       <c r="AK33" s="67"/>
       <c r="AL33" s="60"/>
     </row>
-    <row r="34" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
       <c r="D34" s="64"/>
@@ -3499,7 +3521,7 @@
       <c r="AK34" s="62"/>
       <c r="AL34" s="60"/>
     </row>
-    <row r="35" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="C35" s="56">
         <v>2020</v>
@@ -3555,7 +3577,7 @@
       <c r="AK35" s="62"/>
       <c r="AL35" s="60"/>
     </row>
-    <row r="36" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="59"/>
       <c r="D36" s="60">
@@ -3609,7 +3631,7 @@
       <c r="AK36" s="67"/>
       <c r="AL36" s="64"/>
     </row>
-    <row r="37" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="B37" s="59"/>
       <c r="D37" s="60">
@@ -3663,7 +3685,7 @@
       <c r="AK37" s="62"/>
       <c r="AL37" s="60"/>
     </row>
-    <row r="38" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="60"/>
       <c r="B38" s="59"/>
       <c r="D38" s="60">
@@ -3717,7 +3739,7 @@
       <c r="AK38" s="67"/>
       <c r="AL38" s="64"/>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39" s="60"/>
       <c r="B39" s="59"/>
       <c r="C39">
@@ -3774,7 +3796,7 @@
       <c r="AK39" s="62"/>
       <c r="AL39" s="60"/>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40" s="60"/>
       <c r="B40" s="59"/>
       <c r="C40">
@@ -3816,7 +3838,7 @@
       <c r="AK40" s="84"/>
       <c r="AL40" s="82"/>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41" s="60"/>
       <c r="B41" s="59"/>
       <c r="D41" s="60"/>
@@ -3854,7 +3876,7 @@
       <c r="AK41" s="62"/>
       <c r="AL41" s="60"/>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42" s="60"/>
       <c r="B42" s="59"/>
       <c r="D42" s="60"/>
@@ -3892,7 +3914,7 @@
       <c r="AK42" s="62"/>
       <c r="AL42" s="60"/>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43" s="60"/>
       <c r="B43" s="59"/>
       <c r="D43" s="60"/>
@@ -3930,10 +3952,10 @@
       <c r="AK43" s="62"/>
       <c r="AL43" s="60"/>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B44" s="59"/>
       <c r="C44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D44" s="60"/>
       <c r="E44" s="61"/>
@@ -3984,7 +4006,7 @@
       </c>
       <c r="AL44" s="60"/>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45" s="59"/>
       <c r="B45" s="59"/>
       <c r="D45" s="60"/>
@@ -4010,7 +4032,7 @@
       <c r="Z45" s="62"/>
       <c r="AC45" s="91"/>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46" s="59"/>
       <c r="B46" s="59"/>
       <c r="D46" s="60"/>
@@ -4036,7 +4058,7 @@
       <c r="Z46" s="62"/>
       <c r="AC46" s="91"/>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47" s="59"/>
       <c r="B47" s="59"/>
       <c r="D47" s="60"/>
@@ -4062,7 +4084,7 @@
       <c r="Z47" s="62"/>
       <c r="AC47" s="91"/>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48" s="59"/>
       <c r="B48" s="59"/>
       <c r="D48" s="60"/>
@@ -4099,7 +4121,7 @@
       <c r="AJ48" s="90"/>
       <c r="AK48" s="62"/>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="59"/>
       <c r="B49" s="59"/>
       <c r="D49" s="60"/>
@@ -4131,7 +4153,7 @@
       <c r="AJ49" s="90"/>
       <c r="AK49" s="90"/>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="59"/>
       <c r="D50" s="60"/>
       <c r="E50" s="61"/>
@@ -4162,7 +4184,7 @@
       <c r="AJ50" s="90"/>
       <c r="AK50" s="90"/>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="59"/>
       <c r="D51" s="60"/>
       <c r="E51" s="61"/>
@@ -4193,7 +4215,7 @@
       <c r="AJ51" s="90"/>
       <c r="AK51" s="90"/>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="59"/>
       <c r="D52" s="60"/>
       <c r="E52" s="61"/>
@@ -4224,7 +4246,7 @@
       <c r="AJ52" s="90"/>
       <c r="AK52" s="90"/>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="59"/>
       <c r="D53" s="60"/>
       <c r="E53" s="61"/>
@@ -4269,15 +4291,15 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>791633</xdr:colOff>
+                    <xdr:colOff>790575</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>46567</xdr:rowOff>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>122767</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>